<commit_message>
remove extra sheet from tourney_results.xlsx
</commit_message>
<xml_diff>
--- a/tourney_results.xlsx
+++ b/tourney_results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="0" windowWidth="20260" windowHeight="14740"/>
@@ -10,7 +10,6 @@
     <sheet name="results" sheetId="2" r:id="rId1"/>
     <sheet name="teams" sheetId="4" r:id="rId2"/>
     <sheet name="slot_results" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="224">
   <si>
     <t>#1 Villanova</t>
   </si>
@@ -700,168 +699,6 @@
   </si>
   <si>
     <t>team2</t>
-  </si>
-  <si>
-    <t>2015_1214_1264</t>
-  </si>
-  <si>
-    <t>2015_1140_1279</t>
-  </si>
-  <si>
-    <t>2015_1129_1173</t>
-  </si>
-  <si>
-    <t>2015_1316_1352</t>
-  </si>
-  <si>
-    <t>2015_1248_1437</t>
-  </si>
-  <si>
-    <t>2015_1261_1301</t>
-  </si>
-  <si>
-    <t>2015_1235_1412</t>
-  </si>
-  <si>
-    <t>2015_1186_1207</t>
-  </si>
-  <si>
-    <t>2015_1372_1428</t>
-  </si>
-  <si>
-    <t>2015_1374_1417</t>
-  </si>
-  <si>
-    <t>2015_1214_1246</t>
-  </si>
-  <si>
-    <t>2015_1318_1323</t>
-  </si>
-  <si>
-    <t>2015_1139_1400</t>
-  </si>
-  <si>
-    <t>2015_1153_1345</t>
-  </si>
-  <si>
-    <t>2015_1112_1411</t>
-  </si>
-  <si>
-    <t>2015_1124_1209</t>
-  </si>
-  <si>
-    <t>2015_1217_1314</t>
-  </si>
-  <si>
-    <t>2015_1116_1459</t>
-  </si>
-  <si>
-    <t>2015_1279_1462</t>
-  </si>
-  <si>
-    <t>2015_1326_1433</t>
-  </si>
-  <si>
-    <t>2015_1125_1438</t>
-  </si>
-  <si>
-    <t>2015_1107_1328</t>
-  </si>
-  <si>
-    <t>2015_1257_1414</t>
-  </si>
-  <si>
-    <t>2015_1320_1461</t>
-  </si>
-  <si>
-    <t>2015_1173_1344</t>
-  </si>
-  <si>
-    <t>2015_1208_1277</t>
-  </si>
-  <si>
-    <t>2015_1181_1352</t>
-  </si>
-  <si>
-    <t>2015_1211_1295</t>
-  </si>
-  <si>
-    <t>2015_1172_1234</t>
-  </si>
-  <si>
-    <t>2015_1361_1385</t>
-  </si>
-  <si>
-    <t>2015_1242_1308</t>
-  </si>
-  <si>
-    <t>2015_1268_1434</t>
-  </si>
-  <si>
-    <t>2015_1138_1452</t>
-  </si>
-  <si>
-    <t>2015_1231_1455</t>
-  </si>
-  <si>
-    <t>2015_1157_1458</t>
-  </si>
-  <si>
-    <t>2015_1329_1332</t>
-  </si>
-  <si>
-    <t>2015_1301_1437</t>
-  </si>
-  <si>
-    <t>2015_1412_1417</t>
-  </si>
-  <si>
-    <t>2015_1207_1428</t>
-  </si>
-  <si>
-    <t>2015_1153_1246</t>
-  </si>
-  <si>
-    <t>2015_1139_1323</t>
-  </si>
-  <si>
-    <t>2015_1112_1326</t>
-  </si>
-  <si>
-    <t>2015_1209_1462</t>
-  </si>
-  <si>
-    <t>2015_1116_1314</t>
-  </si>
-  <si>
-    <t>2015_1277_1438</t>
-  </si>
-  <si>
-    <t>2015_1173_1328</t>
-  </si>
-  <si>
-    <t>2015_1257_1320</t>
-  </si>
-  <si>
-    <t>2015_1181_1361</t>
-  </si>
-  <si>
-    <t>2015_1211_1234</t>
-  </si>
-  <si>
-    <t>2015_1242_1455</t>
-  </si>
-  <si>
-    <t>2015_1268_1452</t>
-  </si>
-  <si>
-    <t>2015_1332_1458</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>2015_1112_1462</t>
   </si>
 </sst>
 </file>
@@ -1648,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8438,777 +8275,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C68"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18">
-      <c r="A1" s="40" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>219</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C18" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="C20" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="C22" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="C23" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="C24" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="C25" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="C26" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="C27" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C28" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C29" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="C30" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C31" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="C32" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="C33" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="C34" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="C35" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C36" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="C37" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="C38" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="C39" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="C40" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="C41" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="C42" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="C43" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="C44" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="C45" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="C46" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="C47" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="C48" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="C49" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="C50" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="C51" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="C52" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="C53" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C54" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C55" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C56" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="C57" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C58" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C59" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C60" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C61" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C62" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C63" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C64" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C65" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C66" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C67" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C68" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update tourney_results.xlsx to include Sweet 16 results
</commit_message>
<xml_diff>
--- a/tourney_results.xlsx
+++ b/tourney_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="20260" windowHeight="14740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="2" r:id="rId1"/>
@@ -1485,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4046,10 +4046,12 @@
         <f>IF(G52=1,E52,IF(G52=2,F52,"(not known yet)"))</f>
         <v>#5 West Virginia</v>
       </c>
-      <c r="G54" s="23"/>
+      <c r="G54" s="21">
+        <v>1</v>
+      </c>
       <c r="H54" s="34" t="str">
         <f>IF(G54=1,E54,IF(G54=2,F54,""))</f>
-        <v/>
+        <v>#1 Kentucky</v>
       </c>
       <c r="J54" s="6">
         <f>IFERROR(VLOOKUP(E54,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4069,7 +4071,7 @@
       </c>
       <c r="O54" s="6">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:15" s="6" customFormat="1" ht="13">
@@ -4093,10 +4095,12 @@
         <f>IF(G42=1,E42,IF(G42=2,F42,"(not known yet)"))</f>
         <v>#3 Notre Dame</v>
       </c>
-      <c r="G55" s="7"/>
+      <c r="G55" s="15">
+        <v>2</v>
+      </c>
       <c r="H55" s="30" t="str">
         <f>IF(G55=1,E55,IF(G55=2,F55,""))</f>
-        <v/>
+        <v>#3 Notre Dame</v>
       </c>
       <c r="J55" s="6">
         <f>IFERROR(VLOOKUP(E55,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4116,7 +4120,7 @@
       </c>
       <c r="O55" s="6">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:15" s="6" customFormat="1" ht="13">
@@ -4140,10 +4144,12 @@
         <f>IF(G45=1,E45,IF(G45=2,F45,"(not known yet)"))</f>
         <v>#4 North Carolina</v>
       </c>
-      <c r="G56" s="7"/>
+      <c r="G56" s="15">
+        <v>1</v>
+      </c>
       <c r="H56" s="30" t="str">
         <f>IF(G56=1,E56,IF(G56=2,F56,""))</f>
-        <v/>
+        <v>#1 Wisconsin</v>
       </c>
       <c r="J56" s="6">
         <f>IFERROR(VLOOKUP(E56,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4163,7 +4169,7 @@
       </c>
       <c r="O56" s="6">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:15" s="6" customFormat="1" ht="13">
@@ -4187,10 +4193,12 @@
         <f>IF(G44=1,E44,IF(G44=2,F44,"(not known yet)"))</f>
         <v>#6 Xavier</v>
       </c>
-      <c r="G57" s="7"/>
+      <c r="G57" s="15">
+        <v>1</v>
+      </c>
       <c r="H57" s="30" t="str">
         <f>IF(G57=1,E57,IF(G57=2,F57,""))</f>
-        <v/>
+        <v>#2 Arizona</v>
       </c>
       <c r="J57" s="6">
         <f>IFERROR(VLOOKUP(E57,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4210,7 +4218,7 @@
       </c>
       <c r="O57" s="6">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:15" s="6" customFormat="1" ht="13">
@@ -4234,10 +4242,12 @@
         <f>IF(G48=1,E48,IF(G48=2,F48,"(not known yet)"))</f>
         <v>#4 Louisville</v>
       </c>
-      <c r="G58" s="7"/>
+      <c r="G58" s="15">
+        <v>2</v>
+      </c>
       <c r="H58" s="30" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>#4 Louisville</v>
       </c>
       <c r="J58" s="6">
         <f>IFERROR(VLOOKUP(E58,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4257,7 +4267,7 @@
       </c>
       <c r="O58" s="6">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:15" s="6" customFormat="1" ht="13">
@@ -4281,10 +4291,12 @@
         <f>IF(G47=1,E47,IF(G47=2,F47,"(not known yet)"))</f>
         <v>#3 Oklahoma</v>
       </c>
-      <c r="G59" s="7"/>
+      <c r="G59" s="15">
+        <v>1</v>
+      </c>
       <c r="H59" s="30" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>#7 Michigan St</v>
       </c>
       <c r="J59" s="6">
         <f>IFERROR(VLOOKUP(E59,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4304,7 +4316,7 @@
       </c>
       <c r="O59" s="6">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:15" s="6" customFormat="1" ht="13">
@@ -4328,10 +4340,12 @@
         <f>IF(G40=1,E40,IF(G40=2,F40,"(not known yet)"))</f>
         <v>#5 Utah</v>
       </c>
-      <c r="G60" s="7"/>
+      <c r="G60" s="15">
+        <v>1</v>
+      </c>
       <c r="H60" s="30" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>#1 Duke</v>
       </c>
       <c r="J60" s="6">
         <f>IFERROR(VLOOKUP(E60,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4351,7 +4365,7 @@
       </c>
       <c r="O60" s="6">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:15" s="6" customFormat="1" ht="14" thickBot="1">
@@ -4375,10 +4389,12 @@
         <f>IF(G39=1,E39,IF(G39=2,F39,"(not known yet)"))</f>
         <v>#11 UCLA</v>
       </c>
-      <c r="G61" s="22"/>
+      <c r="G61" s="18">
+        <v>1</v>
+      </c>
       <c r="H61" s="32" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>#2 Gonzaga</v>
       </c>
       <c r="J61" s="6">
         <f>IFERROR(VLOOKUP(E61,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4398,7 +4414,7 @@
       </c>
       <c r="O61" s="6">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:15" s="6" customFormat="1" ht="13">
@@ -4416,24 +4432,24 @@
       </c>
       <c r="E62" s="20" t="str">
         <f>IF(G54=1,E54,IF(G54=2,F54,"(not known yet)"))</f>
-        <v>(not known yet)</v>
+        <v>#1 Kentucky</v>
       </c>
       <c r="F62" s="20" t="str">
         <f>IF(G55=1,E55,IF(G55=2,F55,"(not known yet)"))</f>
-        <v>(not known yet)</v>
+        <v>#3 Notre Dame</v>
       </c>
       <c r="G62" s="23"/>
       <c r="H62" s="34" t="str">
         <f>IF(G62=1,E62,IF(G62=2,F62,""))</f>
         <v/>
       </c>
-      <c r="J62" s="6" t="str">
+      <c r="J62" s="6">
         <f>IFERROR(VLOOKUP(E62,teams!$A$2:$C$69,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K62" s="6" t="str">
+        <v>1246</v>
+      </c>
+      <c r="K62" s="6">
         <f>IFERROR(VLOOKUP(F62,teams!$A$2:$C$69,3,FALSE),"")</f>
-        <v/>
+        <v>1323</v>
       </c>
       <c r="M62" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4441,7 +4457,7 @@
       </c>
       <c r="N62" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>2015_1246_1323</v>
       </c>
       <c r="O62" s="6">
         <f t="shared" si="2"/>
@@ -4463,24 +4479,24 @@
       </c>
       <c r="E63" s="5" t="str">
         <f>IF(G56=1,E56,IF(G56=2,F56,"(not known yet)"))</f>
-        <v>(not known yet)</v>
+        <v>#1 Wisconsin</v>
       </c>
       <c r="F63" s="5" t="str">
         <f>IF(G57=1,E57,IF(G57=2,F57,"(not known yet)"))</f>
-        <v>(not known yet)</v>
+        <v>#2 Arizona</v>
       </c>
       <c r="G63" s="7"/>
       <c r="H63" s="30" t="str">
         <f>IF(G63=1,E63,IF(G63=2,F63,""))</f>
         <v/>
       </c>
-      <c r="J63" s="6" t="str">
+      <c r="J63" s="6">
         <f>IFERROR(VLOOKUP(E63,teams!$A$2:$C$69,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K63" s="6" t="str">
+        <v>1458</v>
+      </c>
+      <c r="K63" s="6">
         <f>IFERROR(VLOOKUP(F63,teams!$A$2:$C$69,3,FALSE),"")</f>
-        <v/>
+        <v>1112</v>
       </c>
       <c r="M63" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4488,7 +4504,7 @@
       </c>
       <c r="N63" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>2015_1112_1458</v>
       </c>
       <c r="O63" s="6">
         <f t="shared" si="2"/>
@@ -4510,24 +4526,24 @@
       </c>
       <c r="E64" s="5" t="str">
         <f>IF(G58=1,E58,IF(G58=2,F58,"(not known yet)"))</f>
-        <v>(not known yet)</v>
+        <v>#4 Louisville</v>
       </c>
       <c r="F64" s="5" t="str">
         <f>IF(G59=1,E59,IF(G59=2,F59,"(not known yet)"))</f>
-        <v>(not known yet)</v>
+        <v>#7 Michigan St</v>
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J64" s="6" t="str">
+      <c r="J64" s="6">
         <f>IFERROR(VLOOKUP(E64,teams!$A$2:$C$69,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K64" s="6" t="str">
+        <v>1257</v>
+      </c>
+      <c r="K64" s="6">
         <f>IFERROR(VLOOKUP(F64,teams!$A$2:$C$69,3,FALSE),"")</f>
-        <v/>
+        <v>1277</v>
       </c>
       <c r="M64" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4535,7 +4551,7 @@
       </c>
       <c r="N64" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>2015_1257_1277</v>
       </c>
       <c r="O64" s="6">
         <f t="shared" si="2"/>
@@ -4557,24 +4573,24 @@
       </c>
       <c r="E65" s="17" t="str">
         <f>IF(G60=1,E60,IF(G60=2,F60,"(not known yet)"))</f>
-        <v>(not known yet)</v>
+        <v>#1 Duke</v>
       </c>
       <c r="F65" s="17" t="str">
         <f>IF(G61=1,E61,IF(G61=2,F61,"(not known yet)"))</f>
-        <v>(not known yet)</v>
+        <v>#2 Gonzaga</v>
       </c>
       <c r="G65" s="22"/>
       <c r="H65" s="32" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J65" s="6" t="str">
+      <c r="J65" s="6">
         <f>IFERROR(VLOOKUP(E65,teams!$A$2:$C$69,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K65" s="6" t="str">
+        <v>1181</v>
+      </c>
+      <c r="K65" s="6">
         <f>IFERROR(VLOOKUP(F65,teams!$A$2:$C$69,3,FALSE),"")</f>
-        <v/>
+        <v>1211</v>
       </c>
       <c r="M65" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4582,7 +4598,7 @@
       </c>
       <c r="N65" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>2015_1181_1211</v>
       </c>
       <c r="O65" s="6">
         <f t="shared" si="2"/>
@@ -7762,33 +7778,33 @@
         <f>results!B58</f>
         <v>R3W1</v>
       </c>
-      <c r="B54" s="13" t="str">
+      <c r="B54" s="13">
         <f>IF(results!G58=1,VLOOKUP(results!E58,teams!A$2:C$69,3,FALSE),IF(results!G58=2,VLOOKUP(results!F58,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1257</v>
       </c>
       <c r="C54" s="14" t="str">
         <f>IF(results!G58=1,VLOOKUP(results!E58,teams!A$2:C$69,1,FALSE),IF(results!G58=2,VLOOKUP(results!F58,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D54" s="13" t="str">
+        <v>#4 Louisville</v>
+      </c>
+      <c r="D54" s="13">
         <f>IF(results!G58=2,VLOOKUP(results!E58,teams!A$2:C$69,3,FALSE),IF(results!G58=1,VLOOKUP(results!F58,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1301</v>
       </c>
       <c r="E54" s="14" t="str">
         <f>IF(results!G58=2,VLOOKUP(results!E58,teams!A$2:C$69,1,FALSE),IF(results!G58=1,VLOOKUP(results!F58,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#8 NC State</v>
       </c>
       <c r="F54" s="14" t="str">
         <f>IF(B54=D54,"",IF(B54&lt;D54,"2015_"&amp;B54&amp;"_"&amp;D54,"2015_"&amp;D54&amp;"_"&amp;B54))</f>
-        <v/>
+        <v>2015_1257_1301</v>
       </c>
       <c r="G54" s="14" t="str">
         <f>IF(B54=D54,"",IF(B54&lt;D54,"1","0"))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H54" s="14" t="str">
         <f>IF(B54=D54,"",IF(B54&lt;D54,"2015_"&amp;B54&amp;"_"&amp;D54&amp;",1","2015_"&amp;D54&amp;"_"&amp;B54&amp;",0"))</f>
-        <v/>
+        <v>2015_1257_1301,1</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -7796,33 +7812,33 @@
         <f>results!B59</f>
         <v>R3W2</v>
       </c>
-      <c r="B55" s="13" t="str">
+      <c r="B55" s="13">
         <f>IF(results!G59=1,VLOOKUP(results!E59,teams!A$2:C$69,3,FALSE),IF(results!G59=2,VLOOKUP(results!F59,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1277</v>
       </c>
       <c r="C55" s="14" t="str">
         <f>IF(results!G59=1,VLOOKUP(results!E59,teams!A$2:C$69,1,FALSE),IF(results!G59=2,VLOOKUP(results!F59,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D55" s="13" t="str">
+        <v>#7 Michigan St</v>
+      </c>
+      <c r="D55" s="13">
         <f>IF(results!G59=2,VLOOKUP(results!E59,teams!A$2:C$69,3,FALSE),IF(results!G59=1,VLOOKUP(results!F59,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1328</v>
       </c>
       <c r="E55" s="14" t="str">
         <f>IF(results!G59=2,VLOOKUP(results!E59,teams!A$2:C$69,1,FALSE),IF(results!G59=1,VLOOKUP(results!F59,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#3 Oklahoma</v>
       </c>
       <c r="F55" s="14" t="str">
         <f>IF(B55=D55,"",IF(B55&lt;D55,"2015_"&amp;B55&amp;"_"&amp;D55,"2015_"&amp;D55&amp;"_"&amp;B55))</f>
-        <v/>
+        <v>2015_1277_1328</v>
       </c>
       <c r="G55" s="14" t="str">
         <f>IF(B55=D55,"",IF(B55&lt;D55,"1","0"))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H55" s="14" t="str">
         <f>IF(B55=D55,"",IF(B55&lt;D55,"2015_"&amp;B55&amp;"_"&amp;D55&amp;",1","2015_"&amp;D55&amp;"_"&amp;B55&amp;",0"))</f>
-        <v/>
+        <v>2015_1277_1328,1</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -7830,33 +7846,33 @@
         <f>results!B60</f>
         <v>R3X1</v>
       </c>
-      <c r="B56" s="13" t="str">
+      <c r="B56" s="13">
         <f>IF(results!G60=1,VLOOKUP(results!E60,teams!A$2:C$69,3,FALSE),IF(results!G60=2,VLOOKUP(results!F60,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1181</v>
       </c>
       <c r="C56" s="14" t="str">
         <f>IF(results!G60=1,VLOOKUP(results!E60,teams!A$2:C$69,1,FALSE),IF(results!G60=2,VLOOKUP(results!F60,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D56" s="13" t="str">
+        <v>#1 Duke</v>
+      </c>
+      <c r="D56" s="13">
         <f>IF(results!G60=2,VLOOKUP(results!E60,teams!A$2:C$69,3,FALSE),IF(results!G60=1,VLOOKUP(results!F60,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1428</v>
       </c>
       <c r="E56" s="14" t="str">
         <f>IF(results!G60=2,VLOOKUP(results!E60,teams!A$2:C$69,1,FALSE),IF(results!G60=1,VLOOKUP(results!F60,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#5 Utah</v>
       </c>
       <c r="F56" s="14" t="str">
         <f>IF(B56=D56,"",IF(B56&lt;D56,"2015_"&amp;B56&amp;"_"&amp;D56,"2015_"&amp;D56&amp;"_"&amp;B56))</f>
-        <v/>
+        <v>2015_1181_1428</v>
       </c>
       <c r="G56" s="14" t="str">
         <f>IF(B56=D56,"",IF(B56&lt;D56,"1","0"))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H56" s="14" t="str">
         <f>IF(B56=D56,"",IF(B56&lt;D56,"2015_"&amp;B56&amp;"_"&amp;D56&amp;",1","2015_"&amp;D56&amp;"_"&amp;B56&amp;",0"))</f>
-        <v/>
+        <v>2015_1181_1428,1</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -7864,33 +7880,33 @@
         <f>results!B61</f>
         <v>R3X2</v>
       </c>
-      <c r="B57" s="13" t="str">
+      <c r="B57" s="13">
         <f>IF(results!G61=1,VLOOKUP(results!E61,teams!A$2:C$69,3,FALSE),IF(results!G61=2,VLOOKUP(results!F61,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1211</v>
       </c>
       <c r="C57" s="14" t="str">
         <f>IF(results!G61=1,VLOOKUP(results!E61,teams!A$2:C$69,1,FALSE),IF(results!G61=2,VLOOKUP(results!F61,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D57" s="13" t="str">
+        <v>#2 Gonzaga</v>
+      </c>
+      <c r="D57" s="13">
         <f>IF(results!G61=2,VLOOKUP(results!E61,teams!A$2:C$69,3,FALSE),IF(results!G61=1,VLOOKUP(results!F61,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1417</v>
       </c>
       <c r="E57" s="14" t="str">
         <f>IF(results!G61=2,VLOOKUP(results!E61,teams!A$2:C$69,1,FALSE),IF(results!G61=1,VLOOKUP(results!F61,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#11 UCLA</v>
       </c>
       <c r="F57" s="14" t="str">
         <f>IF(B57=D57,"",IF(B57&lt;D57,"2015_"&amp;B57&amp;"_"&amp;D57,"2015_"&amp;D57&amp;"_"&amp;B57))</f>
-        <v/>
+        <v>2015_1211_1417</v>
       </c>
       <c r="G57" s="14" t="str">
         <f>IF(B57=D57,"",IF(B57&lt;D57,"1","0"))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H57" s="14" t="str">
         <f>IF(B57=D57,"",IF(B57&lt;D57,"2015_"&amp;B57&amp;"_"&amp;D57&amp;",1","2015_"&amp;D57&amp;"_"&amp;B57&amp;",0"))</f>
-        <v/>
+        <v>2015_1211_1417,1</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -7898,33 +7914,33 @@
         <f>results!B54</f>
         <v>R3Y1</v>
       </c>
-      <c r="B58" s="13" t="str">
+      <c r="B58" s="13">
         <f>IF(results!G54=1,VLOOKUP(results!E54,teams!A$2:C$69,3,FALSE),IF(results!G54=2,VLOOKUP(results!F54,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1246</v>
       </c>
       <c r="C58" s="14" t="str">
         <f>IF(results!G54=1,VLOOKUP(results!E54,teams!A$2:C$69,1,FALSE),IF(results!G54=2,VLOOKUP(results!F54,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D58" s="13" t="str">
+        <v>#1 Kentucky</v>
+      </c>
+      <c r="D58" s="13">
         <f>IF(results!G54=2,VLOOKUP(results!E54,teams!A$2:C$69,3,FALSE),IF(results!G54=1,VLOOKUP(results!F54,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1452</v>
       </c>
       <c r="E58" s="14" t="str">
         <f>IF(results!G54=2,VLOOKUP(results!E54,teams!A$2:C$69,1,FALSE),IF(results!G54=1,VLOOKUP(results!F54,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#5 West Virginia</v>
       </c>
       <c r="F58" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2015_1246_1452</v>
       </c>
       <c r="G58" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H58" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2015_1246_1452,1</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -7932,33 +7948,33 @@
         <f>results!B55</f>
         <v>R3Y2</v>
       </c>
-      <c r="B59" s="13" t="str">
+      <c r="B59" s="13">
         <f>IF(results!G55=1,VLOOKUP(results!E55,teams!A$2:C$69,3,FALSE),IF(results!G55=2,VLOOKUP(results!F55,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1323</v>
       </c>
       <c r="C59" s="14" t="str">
         <f>IF(results!G55=1,VLOOKUP(results!E55,teams!A$2:C$69,1,FALSE),IF(results!G55=2,VLOOKUP(results!F55,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D59" s="13" t="str">
+        <v>#3 Notre Dame</v>
+      </c>
+      <c r="D59" s="13">
         <f>IF(results!G55=2,VLOOKUP(results!E55,teams!A$2:C$69,3,FALSE),IF(results!G55=1,VLOOKUP(results!F55,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1455</v>
       </c>
       <c r="E59" s="14" t="str">
         <f>IF(results!G55=2,VLOOKUP(results!E55,teams!A$2:C$69,1,FALSE),IF(results!G55=1,VLOOKUP(results!F55,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#7 Wichita St</v>
       </c>
       <c r="F59" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2015_1323_1455</v>
       </c>
       <c r="G59" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H59" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2015_1323_1455,1</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -7966,33 +7982,33 @@
         <f>results!B56</f>
         <v>R3Z1</v>
       </c>
-      <c r="B60" s="13" t="str">
+      <c r="B60" s="13">
         <f>IF(results!G56=1,VLOOKUP(results!E56,teams!A$2:C$69,3,FALSE),IF(results!G56=2,VLOOKUP(results!F56,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1458</v>
       </c>
       <c r="C60" s="14" t="str">
         <f>IF(results!G56=1,VLOOKUP(results!E56,teams!A$2:C$69,1,FALSE),IF(results!G56=2,VLOOKUP(results!F56,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D60" s="13" t="str">
+        <v>#1 Wisconsin</v>
+      </c>
+      <c r="D60" s="13">
         <f>IF(results!G56=2,VLOOKUP(results!E56,teams!A$2:C$69,3,FALSE),IF(results!G56=1,VLOOKUP(results!F56,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1314</v>
       </c>
       <c r="E60" s="14" t="str">
         <f>IF(results!G56=2,VLOOKUP(results!E56,teams!A$2:C$69,1,FALSE),IF(results!G56=1,VLOOKUP(results!F56,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#4 North Carolina</v>
       </c>
       <c r="F60" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2015_1314_1458</v>
       </c>
       <c r="G60" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H60" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2015_1314_1458,0</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -8000,33 +8016,33 @@
         <f>results!B57</f>
         <v>R3Z2</v>
       </c>
-      <c r="B61" s="13" t="str">
+      <c r="B61" s="13">
         <f>IF(results!G57=1,VLOOKUP(results!E57,teams!A$2:C$69,3,FALSE),IF(results!G57=2,VLOOKUP(results!F57,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1112</v>
       </c>
       <c r="C61" s="14" t="str">
         <f>IF(results!G57=1,VLOOKUP(results!E57,teams!A$2:C$69,1,FALSE),IF(results!G57=2,VLOOKUP(results!F57,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D61" s="13" t="str">
+        <v>#2 Arizona</v>
+      </c>
+      <c r="D61" s="13">
         <f>IF(results!G57=2,VLOOKUP(results!E57,teams!A$2:C$69,3,FALSE),IF(results!G57=1,VLOOKUP(results!F57,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1462</v>
       </c>
       <c r="E61" s="14" t="str">
         <f>IF(results!G57=2,VLOOKUP(results!E57,teams!A$2:C$69,1,FALSE),IF(results!G57=1,VLOOKUP(results!F57,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#6 Xavier</v>
       </c>
       <c r="F61" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2015_1112_1462</v>
       </c>
       <c r="G61" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H61" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2015_1112_1462,1</v>
       </c>
     </row>
     <row r="62" spans="1:8">

</xml_diff>

<commit_message>
update tourney_results.xlsx to include semifinal results
</commit_message>
<xml_diff>
--- a/tourney_results.xlsx
+++ b/tourney_results.xlsx
@@ -1033,7 +1033,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1085,14 +1085,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1482,7 +1474,7 @@
   <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1501,48 +1493,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="37" thickBot="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="37" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A2" s="32">
+      <c r="A2" s="30">
         <v>42080</v>
       </c>
       <c r="B2" s="18" t="s">
@@ -1563,7 +1555,7 @@
       <c r="G2" s="20">
         <v>1</v>
       </c>
-      <c r="H2" s="33" t="str">
+      <c r="H2" s="31" t="str">
         <f>IF(G2=1,E2,IF(G2=2,F2,""))</f>
         <v>#16 Hampton</v>
       </c>
@@ -1589,7 +1581,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A3" s="28">
+      <c r="A3" s="26">
         <v>42080</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1610,7 +1602,7 @@
       <c r="G3" s="14">
         <v>2</v>
       </c>
-      <c r="H3" s="29" t="str">
+      <c r="H3" s="27" t="str">
         <f>IF(G3=1,E3,IF(G3=2,F3,""))</f>
         <v>#11 Mississippi</v>
       </c>
@@ -1636,7 +1628,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A4" s="28">
+      <c r="A4" s="26">
         <v>42081</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1657,7 +1649,7 @@
       <c r="G4" s="14">
         <v>2</v>
       </c>
-      <c r="H4" s="29" t="str">
+      <c r="H4" s="27" t="str">
         <f>IF(G4=1,E4,IF(G4=2,F4,""))</f>
         <v>#11 Dayton</v>
       </c>
@@ -1683,7 +1675,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="6" customFormat="1" ht="14" thickBot="1">
-      <c r="A5" s="30">
+      <c r="A5" s="28">
         <v>42081</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -1704,7 +1696,7 @@
       <c r="G5" s="17">
         <v>2</v>
       </c>
-      <c r="H5" s="31" t="str">
+      <c r="H5" s="29" t="str">
         <f t="shared" ref="H5:H66" si="3">IF(G5=1,E5,IF(G5=2,F5,""))</f>
         <v>#16 Robert Morris</v>
       </c>
@@ -1730,7 +1722,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A6" s="32">
+      <c r="A6" s="30">
         <v>42082</v>
       </c>
       <c r="B6" s="18" t="s">
@@ -1751,7 +1743,7 @@
       <c r="G6" s="20">
         <v>1</v>
       </c>
-      <c r="H6" s="33" t="str">
+      <c r="H6" s="31" t="str">
         <f t="shared" si="3"/>
         <v>#1 Villanova</v>
       </c>
@@ -1777,7 +1769,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A7" s="28">
+      <c r="A7" s="26">
         <v>42082</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1798,7 +1790,7 @@
       <c r="G7" s="14">
         <v>1</v>
       </c>
-      <c r="H7" s="29" t="str">
+      <c r="H7" s="27" t="str">
         <f t="shared" ref="H7:H21" si="4">IF(G7=1,E7,IF(G7=2,F7,""))</f>
         <v>#8 NC State</v>
       </c>
@@ -1824,7 +1816,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A8" s="28">
+      <c r="A8" s="26">
         <v>42082</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1845,7 +1837,7 @@
       <c r="G8" s="14">
         <v>2</v>
       </c>
-      <c r="H8" s="29" t="str">
+      <c r="H8" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#14 UAB</v>
       </c>
@@ -1871,7 +1863,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A9" s="28">
+      <c r="A9" s="26">
         <v>42082</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1892,7 +1884,7 @@
       <c r="G9" s="14">
         <v>1</v>
       </c>
-      <c r="H9" s="29" t="str">
+      <c r="H9" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#4 Georgetown</v>
       </c>
@@ -1918,7 +1910,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A10" s="28">
+      <c r="A10" s="26">
         <v>42082</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1939,7 +1931,7 @@
       <c r="G10" s="14">
         <v>1</v>
       </c>
-      <c r="H10" s="29" t="str">
+      <c r="H10" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#5 Utah</v>
       </c>
@@ -1965,7 +1957,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A11" s="28">
+      <c r="A11" s="26">
         <v>42082</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1986,7 +1978,7 @@
       <c r="G11" s="14">
         <v>2</v>
       </c>
-      <c r="H11" s="29" t="str">
+      <c r="H11" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#11 UCLA</v>
       </c>
@@ -2012,7 +2004,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A12" s="28">
+      <c r="A12" s="26">
         <v>42082</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2034,7 +2026,7 @@
       <c r="G12" s="14">
         <v>1</v>
       </c>
-      <c r="H12" s="29" t="str">
+      <c r="H12" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#1 Kentucky</v>
       </c>
@@ -2060,7 +2052,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A13" s="28">
+      <c r="A13" s="26">
         <v>42082</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2081,7 +2073,7 @@
       <c r="G13" s="14">
         <v>1</v>
       </c>
-      <c r="H13" s="29" t="str">
+      <c r="H13" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#3 Notre Dame</v>
       </c>
@@ -2107,7 +2099,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A14" s="28">
+      <c r="A14" s="26">
         <v>42082</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2128,7 +2120,7 @@
       <c r="G14" s="14">
         <v>1</v>
       </c>
-      <c r="H14" s="29" t="str">
+      <c r="H14" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#6 Butler</v>
       </c>
@@ -2154,7 +2146,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A15" s="28">
+      <c r="A15" s="26">
         <v>42082</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2175,7 +2167,7 @@
       <c r="G15" s="14">
         <v>1</v>
       </c>
-      <c r="H15" s="29" t="str">
+      <c r="H15" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#8 Cincinnati</v>
       </c>
@@ -2201,7 +2193,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A16" s="28">
+      <c r="A16" s="26">
         <v>42082</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2222,7 +2214,7 @@
       <c r="G16" s="14">
         <v>1</v>
       </c>
-      <c r="H16" s="29" t="str">
+      <c r="H16" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#2 Arizona</v>
       </c>
@@ -2248,7 +2240,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A17" s="28">
+      <c r="A17" s="26">
         <v>42082</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -2269,7 +2261,7 @@
       <c r="G17" s="14">
         <v>2</v>
       </c>
-      <c r="H17" s="29" t="str">
+      <c r="H17" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#14 Georgia St</v>
       </c>
@@ -2295,7 +2287,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A18" s="28">
+      <c r="A18" s="26">
         <v>42082</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -2316,7 +2308,7 @@
       <c r="G18" s="14">
         <v>1</v>
       </c>
-      <c r="H18" s="29" t="str">
+      <c r="H18" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#4 North Carolina</v>
       </c>
@@ -2342,7 +2334,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A19" s="28">
+      <c r="A19" s="26">
         <v>42082</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -2363,7 +2355,7 @@
       <c r="G19" s="14">
         <v>1</v>
       </c>
-      <c r="H19" s="29" t="str">
+      <c r="H19" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#5 Arkansas</v>
       </c>
@@ -2389,7 +2381,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A20" s="28">
+      <c r="A20" s="26">
         <v>42082</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -2411,7 +2403,7 @@
       <c r="G20" s="14">
         <v>1</v>
       </c>
-      <c r="H20" s="29" t="str">
+      <c r="H20" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#6 Xavier</v>
       </c>
@@ -2437,7 +2429,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A21" s="28">
+      <c r="A21" s="26">
         <v>42082</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -2458,7 +2450,7 @@
       <c r="G21" s="14">
         <v>2</v>
       </c>
-      <c r="H21" s="29" t="str">
+      <c r="H21" s="27" t="str">
         <f t="shared" si="4"/>
         <v>#10 Ohio St</v>
       </c>
@@ -2484,7 +2476,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A22" s="28">
+      <c r="A22" s="26">
         <v>42083</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -2505,7 +2497,7 @@
       <c r="G22" s="14">
         <v>1</v>
       </c>
-      <c r="H22" s="29" t="str">
+      <c r="H22" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#2 Virginia</v>
       </c>
@@ -2531,7 +2523,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A23" s="28">
+      <c r="A23" s="26">
         <v>42083</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2552,7 +2544,7 @@
       <c r="G23" s="14">
         <v>1</v>
       </c>
-      <c r="H23" s="29" t="str">
+      <c r="H23" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#3 Oklahoma</v>
       </c>
@@ -2578,7 +2570,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A24" s="28">
+      <c r="A24" s="26">
         <v>42083</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -2599,7 +2591,7 @@
       <c r="G24" s="14">
         <v>1</v>
       </c>
-      <c r="H24" s="29" t="str">
+      <c r="H24" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#4 Louisville</v>
       </c>
@@ -2625,7 +2617,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A25" s="28">
+      <c r="A25" s="26">
         <v>42083</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -2646,7 +2638,7 @@
       <c r="G25" s="14">
         <v>1</v>
       </c>
-      <c r="H25" s="29" t="str">
+      <c r="H25" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#5 Northern Iowa</v>
       </c>
@@ -2672,7 +2664,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A26" s="28">
+      <c r="A26" s="26">
         <v>42083</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -2694,7 +2686,7 @@
       <c r="G26" s="14">
         <v>2</v>
       </c>
-      <c r="H26" s="29" t="str">
+      <c r="H26" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#11 Dayton</v>
       </c>
@@ -2720,7 +2712,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A27" s="28">
+      <c r="A27" s="26">
         <v>42083</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -2741,7 +2733,7 @@
       <c r="G27" s="14">
         <v>1</v>
       </c>
-      <c r="H27" s="29" t="str">
+      <c r="H27" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#7 Michigan St</v>
       </c>
@@ -2767,7 +2759,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A28" s="28">
+      <c r="A28" s="26">
         <v>42083</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -2789,7 +2781,7 @@
       <c r="G28" s="14">
         <v>1</v>
       </c>
-      <c r="H28" s="29" t="str">
+      <c r="H28" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#1 Duke</v>
       </c>
@@ -2815,7 +2807,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A29" s="28">
+      <c r="A29" s="26">
         <v>42083</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -2836,7 +2828,7 @@
       <c r="G29" s="14">
         <v>1</v>
       </c>
-      <c r="H29" s="29" t="str">
+      <c r="H29" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#2 Gonzaga</v>
       </c>
@@ -2862,7 +2854,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A30" s="28">
+      <c r="A30" s="26">
         <v>42083</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -2883,7 +2875,7 @@
       <c r="G30" s="14">
         <v>1</v>
       </c>
-      <c r="H30" s="29" t="str">
+      <c r="H30" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#7 Iowa</v>
       </c>
@@ -2909,7 +2901,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A31" s="28">
+      <c r="A31" s="26">
         <v>42083</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -2930,7 +2922,7 @@
       <c r="G31" s="14">
         <v>1</v>
       </c>
-      <c r="H31" s="29" t="str">
+      <c r="H31" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#8 San Diego St</v>
       </c>
@@ -2956,7 +2948,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A32" s="28">
+      <c r="A32" s="26">
         <v>42083</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -2977,7 +2969,7 @@
       <c r="G32" s="14">
         <v>1</v>
       </c>
-      <c r="H32" s="29" t="str">
+      <c r="H32" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#2 Kansas</v>
       </c>
@@ -3003,7 +2995,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A33" s="28">
+      <c r="A33" s="26">
         <v>42083</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -3024,7 +3016,7 @@
       <c r="G33" s="14">
         <v>1</v>
       </c>
-      <c r="H33" s="29" t="str">
+      <c r="H33" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#4 Maryland</v>
       </c>
@@ -3050,7 +3042,7 @@
       </c>
     </row>
     <row r="34" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A34" s="28">
+      <c r="A34" s="26">
         <v>42083</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -3071,7 +3063,7 @@
       <c r="G34" s="14">
         <v>1</v>
       </c>
-      <c r="H34" s="29" t="str">
+      <c r="H34" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#5 West Virginia</v>
       </c>
@@ -3097,7 +3089,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A35" s="28">
+      <c r="A35" s="26">
         <v>42083</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -3118,7 +3110,7 @@
       <c r="G35" s="14">
         <v>1</v>
       </c>
-      <c r="H35" s="29" t="str">
+      <c r="H35" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#7 Wichita St</v>
       </c>
@@ -3144,7 +3136,7 @@
       </c>
     </row>
     <row r="36" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A36" s="28">
+      <c r="A36" s="26">
         <v>42083</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -3165,7 +3157,7 @@
       <c r="G36" s="14">
         <v>1</v>
       </c>
-      <c r="H36" s="29" t="str">
+      <c r="H36" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#1 Wisconsin</v>
       </c>
@@ -3191,7 +3183,7 @@
       </c>
     </row>
     <row r="37" spans="1:15" s="6" customFormat="1" ht="14" thickBot="1">
-      <c r="A37" s="30">
+      <c r="A37" s="28">
         <v>42083</v>
       </c>
       <c r="B37" s="15" t="s">
@@ -3212,7 +3204,7 @@
       <c r="G37" s="17">
         <v>1</v>
       </c>
-      <c r="H37" s="31" t="str">
+      <c r="H37" s="29" t="str">
         <f t="shared" si="3"/>
         <v>#8 Oregon</v>
       </c>
@@ -3238,7 +3230,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A38" s="32">
+      <c r="A38" s="30">
         <v>42084</v>
       </c>
       <c r="B38" s="18" t="s">
@@ -3261,7 +3253,7 @@
       <c r="G38" s="20">
         <v>2</v>
       </c>
-      <c r="H38" s="33" t="str">
+      <c r="H38" s="31" t="str">
         <f t="shared" si="3"/>
         <v>#8 NC State</v>
       </c>
@@ -3287,7 +3279,7 @@
       </c>
     </row>
     <row r="39" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A39" s="28">
+      <c r="A39" s="26">
         <v>42084</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -3310,7 +3302,7 @@
       <c r="G39" s="14">
         <v>2</v>
       </c>
-      <c r="H39" s="29" t="str">
+      <c r="H39" s="27" t="str">
         <f t="shared" ref="H39:H45" si="5">IF(G39=1,E39,IF(G39=2,F39,""))</f>
         <v>#11 UCLA</v>
       </c>
@@ -3336,7 +3328,7 @@
       </c>
     </row>
     <row r="40" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A40" s="28">
+      <c r="A40" s="26">
         <v>42084</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -3359,7 +3351,7 @@
       <c r="G40" s="14">
         <v>2</v>
       </c>
-      <c r="H40" s="29" t="str">
+      <c r="H40" s="27" t="str">
         <f t="shared" si="5"/>
         <v>#5 Utah</v>
       </c>
@@ -3385,7 +3377,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A41" s="28">
+      <c r="A41" s="26">
         <v>42084</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -3408,7 +3400,7 @@
       <c r="G41" s="14">
         <v>1</v>
       </c>
-      <c r="H41" s="29" t="str">
+      <c r="H41" s="27" t="str">
         <f t="shared" si="5"/>
         <v>#1 Kentucky</v>
       </c>
@@ -3434,7 +3426,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A42" s="28">
+      <c r="A42" s="26">
         <v>42084</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -3457,7 +3449,7 @@
       <c r="G42" s="14">
         <v>1</v>
       </c>
-      <c r="H42" s="29" t="str">
+      <c r="H42" s="27" t="str">
         <f t="shared" si="5"/>
         <v>#3 Notre Dame</v>
       </c>
@@ -3483,7 +3475,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A43" s="28">
+      <c r="A43" s="26">
         <v>42084</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -3506,7 +3498,7 @@
       <c r="G43" s="14">
         <v>1</v>
       </c>
-      <c r="H43" s="29" t="str">
+      <c r="H43" s="27" t="str">
         <f t="shared" si="5"/>
         <v>#2 Arizona</v>
       </c>
@@ -3532,7 +3524,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A44" s="28">
+      <c r="A44" s="26">
         <v>42084</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -3555,7 +3547,7 @@
       <c r="G44" s="14">
         <v>2</v>
       </c>
-      <c r="H44" s="29" t="str">
+      <c r="H44" s="27" t="str">
         <f t="shared" si="5"/>
         <v>#6 Xavier</v>
       </c>
@@ -3581,7 +3573,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A45" s="28">
+      <c r="A45" s="26">
         <v>42084</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -3604,7 +3596,7 @@
       <c r="G45" s="14">
         <v>1</v>
       </c>
-      <c r="H45" s="29" t="str">
+      <c r="H45" s="27" t="str">
         <f t="shared" si="5"/>
         <v>#4 North Carolina</v>
       </c>
@@ -3630,7 +3622,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A46" s="28">
+      <c r="A46" s="26">
         <v>42085</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -3653,7 +3645,7 @@
       <c r="G46" s="14">
         <v>2</v>
       </c>
-      <c r="H46" s="29" t="str">
+      <c r="H46" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#7 Michigan St</v>
       </c>
@@ -3679,7 +3671,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A47" s="28">
+      <c r="A47" s="26">
         <v>42085</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -3702,7 +3694,7 @@
       <c r="G47" s="14">
         <v>1</v>
       </c>
-      <c r="H47" s="29" t="str">
+      <c r="H47" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#3 Oklahoma</v>
       </c>
@@ -3728,7 +3720,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A48" s="28">
+      <c r="A48" s="26">
         <v>42085</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -3751,7 +3743,7 @@
       <c r="G48" s="14">
         <v>1</v>
       </c>
-      <c r="H48" s="29" t="str">
+      <c r="H48" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#4 Louisville</v>
       </c>
@@ -3777,7 +3769,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A49" s="28">
+      <c r="A49" s="26">
         <v>42085</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -3800,7 +3792,7 @@
       <c r="G49" s="14">
         <v>1</v>
       </c>
-      <c r="H49" s="29" t="str">
+      <c r="H49" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#1 Duke</v>
       </c>
@@ -3826,7 +3818,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A50" s="28">
+      <c r="A50" s="26">
         <v>42085</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -3849,7 +3841,7 @@
       <c r="G50" s="14">
         <v>1</v>
       </c>
-      <c r="H50" s="29" t="str">
+      <c r="H50" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#2 Gonzaga</v>
       </c>
@@ -3875,7 +3867,7 @@
       </c>
     </row>
     <row r="51" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A51" s="28">
+      <c r="A51" s="26">
         <v>42085</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -3898,7 +3890,7 @@
       <c r="G51" s="14">
         <v>2</v>
       </c>
-      <c r="H51" s="29" t="str">
+      <c r="H51" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#7 Wichita St</v>
       </c>
@@ -3924,7 +3916,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A52" s="28">
+      <c r="A52" s="26">
         <v>42085</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -3947,7 +3939,7 @@
       <c r="G52" s="14">
         <v>2</v>
       </c>
-      <c r="H52" s="29" t="str">
+      <c r="H52" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#5 West Virginia</v>
       </c>
@@ -3973,7 +3965,7 @@
       </c>
     </row>
     <row r="53" spans="1:15" s="6" customFormat="1" ht="14" thickBot="1">
-      <c r="A53" s="30">
+      <c r="A53" s="28">
         <v>42085</v>
       </c>
       <c r="B53" s="15" t="s">
@@ -3996,7 +3988,7 @@
       <c r="G53" s="17">
         <v>1</v>
       </c>
-      <c r="H53" s="31" t="str">
+      <c r="H53" s="29" t="str">
         <f t="shared" si="3"/>
         <v>#1 Wisconsin</v>
       </c>
@@ -4022,7 +4014,7 @@
       </c>
     </row>
     <row r="54" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A54" s="32">
+      <c r="A54" s="30">
         <v>42089</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -4045,7 +4037,7 @@
       <c r="G54" s="20">
         <v>1</v>
       </c>
-      <c r="H54" s="33" t="str">
+      <c r="H54" s="31" t="str">
         <f>IF(G54=1,E54,IF(G54=2,F54,""))</f>
         <v>#1 Kentucky</v>
       </c>
@@ -4071,7 +4063,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A55" s="28">
+      <c r="A55" s="26">
         <v>42089</v>
       </c>
       <c r="B55" s="4" t="s">
@@ -4094,7 +4086,7 @@
       <c r="G55" s="14">
         <v>2</v>
       </c>
-      <c r="H55" s="29" t="str">
+      <c r="H55" s="27" t="str">
         <f>IF(G55=1,E55,IF(G55=2,F55,""))</f>
         <v>#3 Notre Dame</v>
       </c>
@@ -4120,7 +4112,7 @@
       </c>
     </row>
     <row r="56" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A56" s="28">
+      <c r="A56" s="26">
         <v>42089</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -4143,7 +4135,7 @@
       <c r="G56" s="14">
         <v>1</v>
       </c>
-      <c r="H56" s="29" t="str">
+      <c r="H56" s="27" t="str">
         <f>IF(G56=1,E56,IF(G56=2,F56,""))</f>
         <v>#1 Wisconsin</v>
       </c>
@@ -4169,7 +4161,7 @@
       </c>
     </row>
     <row r="57" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A57" s="28">
+      <c r="A57" s="26">
         <v>42089</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -4192,7 +4184,7 @@
       <c r="G57" s="14">
         <v>1</v>
       </c>
-      <c r="H57" s="29" t="str">
+      <c r="H57" s="27" t="str">
         <f>IF(G57=1,E57,IF(G57=2,F57,""))</f>
         <v>#2 Arizona</v>
       </c>
@@ -4218,7 +4210,7 @@
       </c>
     </row>
     <row r="58" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A58" s="28">
+      <c r="A58" s="26">
         <v>42090</v>
       </c>
       <c r="B58" s="4" t="s">
@@ -4241,7 +4233,7 @@
       <c r="G58" s="14">
         <v>2</v>
       </c>
-      <c r="H58" s="29" t="str">
+      <c r="H58" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#4 Louisville</v>
       </c>
@@ -4267,7 +4259,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A59" s="28">
+      <c r="A59" s="26">
         <v>42090</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -4290,7 +4282,7 @@
       <c r="G59" s="14">
         <v>1</v>
       </c>
-      <c r="H59" s="29" t="str">
+      <c r="H59" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#7 Michigan St</v>
       </c>
@@ -4316,7 +4308,7 @@
       </c>
     </row>
     <row r="60" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A60" s="28">
+      <c r="A60" s="26">
         <v>42090</v>
       </c>
       <c r="B60" s="4" t="s">
@@ -4339,7 +4331,7 @@
       <c r="G60" s="14">
         <v>1</v>
       </c>
-      <c r="H60" s="29" t="str">
+      <c r="H60" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#1 Duke</v>
       </c>
@@ -4365,7 +4357,7 @@
       </c>
     </row>
     <row r="61" spans="1:15" s="6" customFormat="1" ht="14" thickBot="1">
-      <c r="A61" s="30">
+      <c r="A61" s="28">
         <v>42090</v>
       </c>
       <c r="B61" s="15" t="s">
@@ -4388,7 +4380,7 @@
       <c r="G61" s="17">
         <v>1</v>
       </c>
-      <c r="H61" s="31" t="str">
+      <c r="H61" s="29" t="str">
         <f t="shared" si="3"/>
         <v>#2 Gonzaga</v>
       </c>
@@ -4414,7 +4406,7 @@
       </c>
     </row>
     <row r="62" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A62" s="32">
+      <c r="A62" s="30">
         <v>42091</v>
       </c>
       <c r="B62" s="18" t="s">
@@ -4437,7 +4429,7 @@
       <c r="G62" s="20">
         <v>1</v>
       </c>
-      <c r="H62" s="33" t="str">
+      <c r="H62" s="31" t="str">
         <f>IF(G62=1,E62,IF(G62=2,F62,""))</f>
         <v>#1 Kentucky</v>
       </c>
@@ -4463,7 +4455,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A63" s="28">
+      <c r="A63" s="26">
         <v>42091</v>
       </c>
       <c r="B63" s="4" t="s">
@@ -4486,7 +4478,7 @@
       <c r="G63" s="14">
         <v>1</v>
       </c>
-      <c r="H63" s="29" t="str">
+      <c r="H63" s="27" t="str">
         <f>IF(G63=1,E63,IF(G63=2,F63,""))</f>
         <v>#1 Wisconsin</v>
       </c>
@@ -4512,7 +4504,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A64" s="28">
+      <c r="A64" s="26">
         <v>42092</v>
       </c>
       <c r="B64" s="4" t="s">
@@ -4535,7 +4527,7 @@
       <c r="G64" s="14">
         <v>2</v>
       </c>
-      <c r="H64" s="29" t="str">
+      <c r="H64" s="27" t="str">
         <f t="shared" si="3"/>
         <v>#7 Michigan St</v>
       </c>
@@ -4561,7 +4553,7 @@
       </c>
     </row>
     <row r="65" spans="1:15" s="6" customFormat="1" ht="14" thickBot="1">
-      <c r="A65" s="30">
+      <c r="A65" s="28">
         <v>42092</v>
       </c>
       <c r="B65" s="15" t="s">
@@ -4584,7 +4576,7 @@
       <c r="G65" s="17">
         <v>1</v>
       </c>
-      <c r="H65" s="31" t="str">
+      <c r="H65" s="29" t="str">
         <f t="shared" si="3"/>
         <v>#1 Duke</v>
       </c>
@@ -4610,7 +4602,7 @@
       </c>
     </row>
     <row r="66" spans="1:15" s="6" customFormat="1" ht="13">
-      <c r="A66" s="32">
+      <c r="A66" s="30">
         <v>42098</v>
       </c>
       <c r="B66" s="18" t="s">
@@ -4630,10 +4622,12 @@
         <f>IF(G65=1,E65,IF(G65=2,F65,"(not known yet)"))</f>
         <v>#1 Duke</v>
       </c>
-      <c r="G66" s="22"/>
-      <c r="H66" s="33" t="str">
+      <c r="G66" s="20">
+        <v>2</v>
+      </c>
+      <c r="H66" s="31" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>#1 Duke</v>
       </c>
       <c r="J66" s="6">
         <f>IFERROR(VLOOKUP(E66,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4653,11 +4647,11 @@
       </c>
       <c r="O66" s="6">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:15" s="6" customFormat="1" ht="14" thickBot="1">
-      <c r="A67" s="30">
+      <c r="A67" s="28">
         <v>42098</v>
       </c>
       <c r="B67" s="15" t="s">
@@ -4677,10 +4671,12 @@
         <f>IF(G63=1,E63,IF(G63=2,F63,"(not known yet)"))</f>
         <v>#1 Wisconsin</v>
       </c>
-      <c r="G67" s="21"/>
-      <c r="H67" s="31" t="str">
+      <c r="G67" s="17">
+        <v>2</v>
+      </c>
+      <c r="H67" s="29" t="str">
         <f t="shared" ref="H67:H68" si="6">IF(G67=1,E67,IF(G67=2,F67,""))</f>
-        <v/>
+        <v>#1 Wisconsin</v>
       </c>
       <c r="J67" s="6">
         <f>IFERROR(VLOOKUP(E67,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4700,42 +4696,42 @@
       </c>
       <c r="O67" s="6">
         <f t="shared" ref="O67:O68" si="9">IFERROR(IF(TEXT(INDEX(J67:K67,1,G67),"0")=MID(N67,6,4),1,0),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:15" s="6" customFormat="1" ht="14" thickBot="1">
-      <c r="A68" s="34">
+      <c r="A68" s="32">
         <v>42100</v>
       </c>
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="C68" s="36" t="s">
+      <c r="C68" s="34" t="s">
         <v>200</v>
       </c>
-      <c r="D68" s="36" t="s">
+      <c r="D68" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="E68" s="36" t="str">
+      <c r="E68" s="34" t="str">
         <f>IF(G66=1,E66,IF(G66=2,F66,"(not known yet)"))</f>
-        <v>(not known yet)</v>
-      </c>
-      <c r="F68" s="36" t="str">
+        <v>#1 Duke</v>
+      </c>
+      <c r="F68" s="34" t="str">
         <f>IF(G67=1,E67,IF(G67=2,F67,"(not known yet)"))</f>
-        <v>(not known yet)</v>
-      </c>
-      <c r="G68" s="37"/>
-      <c r="H68" s="38" t="str">
+        <v>#1 Wisconsin</v>
+      </c>
+      <c r="G68" s="35"/>
+      <c r="H68" s="36" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="J68" s="6" t="str">
+      <c r="J68" s="6">
         <f>IFERROR(VLOOKUP(E68,teams!$A$2:$C$69,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K68" s="6" t="str">
+        <v>1181</v>
+      </c>
+      <c r="K68" s="6">
         <f>IFERROR(VLOOKUP(F68,teams!$A$2:$C$69,3,FALSE),"")</f>
-        <v/>
+        <v>1458</v>
       </c>
       <c r="M68" s="6" t="str">
         <f t="shared" si="7"/>
@@ -4743,7 +4739,7 @@
       </c>
       <c r="N68" s="6" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>2015_1181_1458</v>
       </c>
       <c r="O68" s="6">
         <f t="shared" si="9"/>
@@ -8190,33 +8186,33 @@
         <f>results!B66</f>
         <v>R5WX</v>
       </c>
-      <c r="B66" s="12" t="str">
+      <c r="B66" s="12">
         <f>IF(results!G66=1,VLOOKUP(results!E66,teams!A$2:C$69,3,FALSE),IF(results!G66=2,VLOOKUP(results!F66,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1181</v>
       </c>
       <c r="C66" s="13" t="str">
         <f>IF(results!G66=1,VLOOKUP(results!E66,teams!A$2:C$69,1,FALSE),IF(results!G66=2,VLOOKUP(results!F66,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D66" s="12" t="str">
+        <v>#1 Duke</v>
+      </c>
+      <c r="D66" s="12">
         <f>IF(results!G66=2,VLOOKUP(results!E66,teams!A$2:C$69,3,FALSE),IF(results!G66=1,VLOOKUP(results!F66,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1277</v>
       </c>
       <c r="E66" s="13" t="str">
         <f>IF(results!G66=2,VLOOKUP(results!E66,teams!A$2:C$69,1,FALSE),IF(results!G66=1,VLOOKUP(results!F66,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#7 Michigan St</v>
       </c>
       <c r="F66" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2015_1181_1277</v>
       </c>
       <c r="G66" s="13" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H66" s="13" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2015_1181_1277,1</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -8224,33 +8220,33 @@
         <f>results!B67</f>
         <v>R5YZ</v>
       </c>
-      <c r="B67" s="12" t="str">
+      <c r="B67" s="12">
         <f>IF(results!G67=1,VLOOKUP(results!E67,teams!A$2:C$69,3,FALSE),IF(results!G67=2,VLOOKUP(results!F67,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1458</v>
       </c>
       <c r="C67" s="13" t="str">
         <f>IF(results!G67=1,VLOOKUP(results!E67,teams!A$2:C$69,1,FALSE),IF(results!G67=2,VLOOKUP(results!F67,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D67" s="12" t="str">
+        <v>#1 Wisconsin</v>
+      </c>
+      <c r="D67" s="12">
         <f>IF(results!G67=2,VLOOKUP(results!E67,teams!A$2:C$69,3,FALSE),IF(results!G67=1,VLOOKUP(results!F67,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1246</v>
       </c>
       <c r="E67" s="13" t="str">
         <f>IF(results!G67=2,VLOOKUP(results!E67,teams!A$2:C$69,1,FALSE),IF(results!G67=1,VLOOKUP(results!F67,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#1 Kentucky</v>
       </c>
       <c r="F67" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2015_1246_1458</v>
       </c>
       <c r="G67" s="13" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H67" s="13" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2015_1246_1458,0</v>
       </c>
     </row>
     <row r="68" spans="1:8">

</xml_diff>

<commit_message>
update tourney_results.xlsx to include championship game result
</commit_message>
<xml_diff>
--- a/tourney_results.xlsx
+++ b/tourney_results.xlsx
@@ -744,7 +744,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,12 +760,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,7 +1062,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1076,7 +1070,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1084,7 +1078,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1122,13 +1116,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -1474,7 +1468,7 @@
   <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1517,19 +1511,19 @@
       <c r="H1" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="M1" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="O1" s="36" t="s">
         <v>220</v>
       </c>
     </row>
@@ -4720,10 +4714,12 @@
         <f>IF(G67=1,E67,IF(G67=2,F67,"(not known yet)"))</f>
         <v>#1 Wisconsin</v>
       </c>
-      <c r="G68" s="35"/>
-      <c r="H68" s="36" t="str">
+      <c r="G68" s="37">
+        <v>1</v>
+      </c>
+      <c r="H68" s="35" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#1 Duke</v>
       </c>
       <c r="J68" s="6">
         <f>IFERROR(VLOOKUP(E68,teams!$A$2:$C$69,3,FALSE),"")</f>
@@ -4743,7 +4739,7 @@
       </c>
       <c r="O68" s="6">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8254,33 +8250,33 @@
         <f>results!B68</f>
         <v>R6CH</v>
       </c>
-      <c r="B68" s="12" t="str">
+      <c r="B68" s="12">
         <f>IF(results!G68=1,VLOOKUP(results!E68,teams!A$2:C$69,3,FALSE),IF(results!G68=2,VLOOKUP(results!F68,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1181</v>
       </c>
       <c r="C68" s="13" t="str">
         <f>IF(results!G68=1,VLOOKUP(results!E68,teams!A$2:C$69,1,FALSE),IF(results!G68=2,VLOOKUP(results!F68,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
-      </c>
-      <c r="D68" s="12" t="str">
+        <v>#1 Duke</v>
+      </c>
+      <c r="D68" s="12">
         <f>IF(results!G68=2,VLOOKUP(results!E68,teams!A$2:C$69,3,FALSE),IF(results!G68=1,VLOOKUP(results!F68,teams!A$2:C$69,3,FALSE),""))</f>
-        <v/>
+        <v>1458</v>
       </c>
       <c r="E68" s="13" t="str">
         <f>IF(results!G68=2,VLOOKUP(results!E68,teams!A$2:C$69,1,FALSE),IF(results!G68=1,VLOOKUP(results!F68,teams!A$2:C$69,1,FALSE),""))</f>
-        <v/>
+        <v>#1 Wisconsin</v>
       </c>
       <c r="F68" s="13" t="str">
         <f t="shared" ref="F68" si="6">IF(B68=D68,"",IF(B68&lt;D68,"2015_"&amp;B68&amp;"_"&amp;D68,"2015_"&amp;D68&amp;"_"&amp;B68))</f>
-        <v/>
+        <v>2015_1181_1458</v>
       </c>
       <c r="G68" s="13" t="str">
         <f t="shared" ref="G68" si="7">IF(B68=D68,"",IF(B68&lt;D68,"1","0"))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H68" s="13" t="str">
         <f t="shared" ref="H68" si="8">IF(B68=D68,"",IF(B68&lt;D68,"2015_"&amp;B68&amp;"_"&amp;D68&amp;",1","2015_"&amp;D68&amp;"_"&amp;B68&amp;",0"))</f>
-        <v/>
+        <v>2015_1181_1458,1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tourney_results.xlsx to include all 2016 tournament results
</commit_message>
<xml_diff>
--- a/tourney_results.xlsx
+++ b/tourney_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30080" windowHeight="24700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="2" r:id="rId1"/>
@@ -1564,7 +1564,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -4245,10 +4247,12 @@
         <f>VLOOKUP(D54,$B$6:$H53,7,FALSE)</f>
         <v>#5 Maryland</v>
       </c>
-      <c r="G54" s="20"/>
+      <c r="G54" s="20">
+        <v>1</v>
+      </c>
       <c r="H54" s="31" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
+        <v>#1 Kansas</v>
       </c>
       <c r="J54" s="6">
         <f>IFERROR(VLOOKUP(E54,teams!$B$2:$C$69,2,FALSE),"")</f>
@@ -4268,7 +4272,7 @@
       </c>
       <c r="O54" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Q54" s="39"/>
     </row>
@@ -4293,10 +4297,12 @@
         <f>VLOOKUP(D55,$B$6:$H54,7,FALSE)</f>
         <v>#3 Miami FL</v>
       </c>
-      <c r="G55" s="14"/>
+      <c r="G55" s="14">
+        <v>1</v>
+      </c>
       <c r="H55" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
+        <v>#2 Villanova</v>
       </c>
       <c r="J55" s="6">
         <f>IFERROR(VLOOKUP(E55,teams!$B$2:$C$69,2,FALSE),"")</f>
@@ -4316,7 +4322,7 @@
       </c>
       <c r="O55" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q55" s="39"/>
     </row>
@@ -4341,10 +4347,12 @@
         <f>VLOOKUP(D56,$B$6:$H55,7,FALSE)</f>
         <v>#4 Duke</v>
       </c>
-      <c r="G56" s="14"/>
+      <c r="G56" s="14">
+        <v>1</v>
+      </c>
       <c r="H56" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
+        <v>#1 Oregon</v>
       </c>
       <c r="J56" s="6">
         <f>IFERROR(VLOOKUP(E56,teams!$B$2:$C$69,2,FALSE),"")</f>
@@ -4364,7 +4372,7 @@
       </c>
       <c r="O56" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q56" s="39"/>
     </row>
@@ -4389,10 +4397,12 @@
         <f>VLOOKUP(D57,$B$6:$H56,7,FALSE)</f>
         <v>#3 Texas A&amp;M</v>
       </c>
-      <c r="G57" s="14"/>
+      <c r="G57" s="14">
+        <v>1</v>
+      </c>
       <c r="H57" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
+        <v>#2 Oklahoma</v>
       </c>
       <c r="J57" s="6">
         <f>IFERROR(VLOOKUP(E57,teams!$B$2:$C$69,2,FALSE),"")</f>
@@ -4412,7 +4422,7 @@
       </c>
       <c r="O57" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Q57" s="39"/>
     </row>
@@ -4437,10 +4447,12 @@
         <f>VLOOKUP(D58,$B$6:$H57,7,FALSE)</f>
         <v>#5 Indiana</v>
       </c>
-      <c r="G58" s="14"/>
+      <c r="G58" s="14">
+        <v>1</v>
+      </c>
       <c r="H58" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
+        <v>#1 North Carolina</v>
       </c>
       <c r="J58" s="6">
         <f>IFERROR(VLOOKUP(E58,teams!$B$2:$C$69,2,FALSE),"")</f>
@@ -4460,7 +4472,7 @@
       </c>
       <c r="O58" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q58" s="39"/>
     </row>
@@ -4485,10 +4497,12 @@
         <f>VLOOKUP(D59,$B$6:$H58,7,FALSE)</f>
         <v>#6 Notre Dame</v>
       </c>
-      <c r="G59" s="14"/>
+      <c r="G59" s="14">
+        <v>2</v>
+      </c>
       <c r="H59" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
+        <v>#6 Notre Dame</v>
       </c>
       <c r="J59" s="6">
         <f>IFERROR(VLOOKUP(E59,teams!$B$2:$C$69,2,FALSE),"")</f>
@@ -4508,7 +4522,7 @@
       </c>
       <c r="O59" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Q59" s="39"/>
     </row>
@@ -4533,10 +4547,12 @@
         <f>VLOOKUP(D60,$B$6:$H59,7,FALSE)</f>
         <v>#4 Iowa St</v>
       </c>
-      <c r="G60" s="14"/>
+      <c r="G60" s="14">
+        <v>1</v>
+      </c>
       <c r="H60" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
+        <v>#1 Virginia</v>
       </c>
       <c r="J60" s="6">
         <f>IFERROR(VLOOKUP(E60,teams!$B$2:$C$69,2,FALSE),"")</f>
@@ -4556,7 +4572,7 @@
       </c>
       <c r="O60" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q60" s="39"/>
     </row>
@@ -4581,10 +4597,12 @@
         <f>VLOOKUP(D61,$B$6:$H60,7,FALSE)</f>
         <v>#11 Gonzaga</v>
       </c>
-      <c r="G61" s="17"/>
+      <c r="G61" s="17">
+        <v>1</v>
+      </c>
       <c r="H61" s="29" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
+        <v>#10 Syracuse</v>
       </c>
       <c r="J61" s="6">
         <f>IFERROR(VLOOKUP(E61,teams!$B$2:$C$69,2,FALSE),"")</f>
@@ -4604,7 +4622,7 @@
       </c>
       <c r="O61" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q61" s="39"/>
     </row>
@@ -4623,24 +4641,26 @@
       </c>
       <c r="E62" s="19" t="str">
         <f>VLOOKUP(C62,$B$6:$H61,7,FALSE)</f>
-        <v>TBD</v>
+        <v>#1 Kansas</v>
       </c>
       <c r="F62" s="19" t="str">
         <f>VLOOKUP(D62,$B$6:$H61,7,FALSE)</f>
-        <v>TBD</v>
-      </c>
-      <c r="G62" s="20"/>
+        <v>#2 Villanova</v>
+      </c>
+      <c r="G62" s="20">
+        <v>2</v>
+      </c>
       <c r="H62" s="31" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
-      </c>
-      <c r="J62" s="6" t="str">
+        <v>#2 Villanova</v>
+      </c>
+      <c r="J62" s="6">
         <f>IFERROR(VLOOKUP(E62,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K62" s="6" t="str">
+        <v>1242</v>
+      </c>
+      <c r="K62" s="6">
         <f>IFERROR(VLOOKUP(F62,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
+        <v>1437</v>
       </c>
       <c r="M62" s="6" t="str">
         <f t="shared" si="1"/>
@@ -4648,11 +4668,11 @@
       </c>
       <c r="N62" s="6" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2016_1242_1437</v>
       </c>
       <c r="O62" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q62" s="39"/>
     </row>
@@ -4671,24 +4691,26 @@
       </c>
       <c r="E63" s="5" t="str">
         <f>VLOOKUP(C63,$B$6:$H62,7,FALSE)</f>
-        <v>TBD</v>
+        <v>#1 Oregon</v>
       </c>
       <c r="F63" s="5" t="str">
         <f>VLOOKUP(D63,$B$6:$H62,7,FALSE)</f>
-        <v>TBD</v>
-      </c>
-      <c r="G63" s="14"/>
+        <v>#2 Oklahoma</v>
+      </c>
+      <c r="G63" s="14">
+        <v>2</v>
+      </c>
       <c r="H63" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
-      </c>
-      <c r="J63" s="6" t="str">
+        <v>#2 Oklahoma</v>
+      </c>
+      <c r="J63" s="6">
         <f>IFERROR(VLOOKUP(E63,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K63" s="6" t="str">
+        <v>1332</v>
+      </c>
+      <c r="K63" s="6">
         <f>IFERROR(VLOOKUP(F63,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
+        <v>1328</v>
       </c>
       <c r="M63" s="6" t="str">
         <f t="shared" si="1"/>
@@ -4696,11 +4718,11 @@
       </c>
       <c r="N63" s="6" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2016_1328_1332</v>
       </c>
       <c r="O63" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Q63" s="39"/>
     </row>
@@ -4719,24 +4741,26 @@
       </c>
       <c r="E64" s="5" t="str">
         <f>VLOOKUP(C64,$B$6:$H63,7,FALSE)</f>
-        <v>TBD</v>
+        <v>#1 North Carolina</v>
       </c>
       <c r="F64" s="5" t="str">
         <f>VLOOKUP(D64,$B$6:$H63,7,FALSE)</f>
-        <v>TBD</v>
-      </c>
-      <c r="G64" s="14"/>
+        <v>#6 Notre Dame</v>
+      </c>
+      <c r="G64" s="14">
+        <v>1</v>
+      </c>
       <c r="H64" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
-      </c>
-      <c r="J64" s="6" t="str">
+        <v>#1 North Carolina</v>
+      </c>
+      <c r="J64" s="6">
         <f>IFERROR(VLOOKUP(E64,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K64" s="6" t="str">
+        <v>1314</v>
+      </c>
+      <c r="K64" s="6">
         <f>IFERROR(VLOOKUP(F64,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
+        <v>1323</v>
       </c>
       <c r="M64" s="6" t="str">
         <f t="shared" si="1"/>
@@ -4744,11 +4768,11 @@
       </c>
       <c r="N64" s="6" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2016_1314_1323</v>
       </c>
       <c r="O64" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Q64" s="39"/>
     </row>
@@ -4767,24 +4791,26 @@
       </c>
       <c r="E65" s="16" t="str">
         <f>VLOOKUP(C65,$B$6:$H64,7,FALSE)</f>
-        <v>TBD</v>
+        <v>#1 Virginia</v>
       </c>
       <c r="F65" s="16" t="str">
         <f>VLOOKUP(D65,$B$6:$H64,7,FALSE)</f>
-        <v>TBD</v>
-      </c>
-      <c r="G65" s="17"/>
+        <v>#10 Syracuse</v>
+      </c>
+      <c r="G65" s="17">
+        <v>2</v>
+      </c>
       <c r="H65" s="29" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
-      </c>
-      <c r="J65" s="6" t="str">
+        <v>#10 Syracuse</v>
+      </c>
+      <c r="J65" s="6">
         <f>IFERROR(VLOOKUP(E65,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K65" s="6" t="str">
+        <v>1438</v>
+      </c>
+      <c r="K65" s="6">
         <f>IFERROR(VLOOKUP(F65,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
+        <v>1393</v>
       </c>
       <c r="M65" s="6" t="str">
         <f t="shared" si="1"/>
@@ -4792,11 +4818,11 @@
       </c>
       <c r="N65" s="6" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2016_1393_1438</v>
       </c>
       <c r="O65" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Q65" s="39"/>
     </row>
@@ -4815,24 +4841,26 @@
       </c>
       <c r="E66" s="19" t="str">
         <f>VLOOKUP(C66,$B$6:$H65,7,FALSE)</f>
-        <v>TBD</v>
+        <v>#1 North Carolina</v>
       </c>
       <c r="F66" s="19" t="str">
         <f>VLOOKUP(D66,$B$6:$H65,7,FALSE)</f>
-        <v>TBD</v>
-      </c>
-      <c r="G66" s="20"/>
+        <v>#10 Syracuse</v>
+      </c>
+      <c r="G66" s="20">
+        <v>1</v>
+      </c>
       <c r="H66" s="31" t="str">
         <f t="shared" si="0"/>
-        <v>TBD</v>
-      </c>
-      <c r="J66" s="6" t="str">
+        <v>#1 North Carolina</v>
+      </c>
+      <c r="J66" s="6">
         <f>IFERROR(VLOOKUP(E66,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K66" s="6" t="str">
+        <v>1314</v>
+      </c>
+      <c r="K66" s="6">
         <f>IFERROR(VLOOKUP(F66,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
+        <v>1393</v>
       </c>
       <c r="M66" s="6" t="str">
         <f t="shared" si="1"/>
@@ -4840,11 +4868,11 @@
       </c>
       <c r="N66" s="6" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2016_1314_1393</v>
       </c>
       <c r="O66" s="6">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Q66" s="39"/>
     </row>
@@ -4863,24 +4891,26 @@
       </c>
       <c r="E67" s="16" t="str">
         <f>VLOOKUP(C67,$B$6:$H66,7,FALSE)</f>
-        <v>TBD</v>
+        <v>#2 Villanova</v>
       </c>
       <c r="F67" s="16" t="str">
         <f>VLOOKUP(D67,$B$6:$H66,7,FALSE)</f>
-        <v>TBD</v>
-      </c>
-      <c r="G67" s="17"/>
+        <v>#2 Oklahoma</v>
+      </c>
+      <c r="G67" s="17">
+        <v>1</v>
+      </c>
       <c r="H67" s="29" t="str">
         <f t="shared" ref="H67:H68" si="4">IF(G67=1,E67,IF(G67=2,F67,"TBD"))</f>
-        <v>TBD</v>
-      </c>
-      <c r="J67" s="6" t="str">
+        <v>#2 Villanova</v>
+      </c>
+      <c r="J67" s="6">
         <f>IFERROR(VLOOKUP(E67,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K67" s="6" t="str">
+        <v>1437</v>
+      </c>
+      <c r="K67" s="6">
         <f>IFERROR(VLOOKUP(F67,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
+        <v>1328</v>
       </c>
       <c r="M67" s="6" t="str">
         <f t="shared" ref="M67:M68" si="5">B67</f>
@@ -4888,11 +4918,11 @@
       </c>
       <c r="N67" s="6" t="str">
         <f t="shared" ref="N67:N68" si="6">IF(AND(J67&lt;&gt;"",K67&lt;&gt;""),IF(J67&lt;K67,"2016_"&amp;J67&amp;"_"&amp;K67,"2016_"&amp;K67&amp;"_"&amp;J67),"")</f>
-        <v/>
+        <v>2016_1328_1437</v>
       </c>
       <c r="O67" s="6">
         <f t="shared" ref="O67:O68" si="7">IFERROR(IF(TEXT(INDEX(J67:K67,1,G67),"0")=MID(N67,6,4),1,0),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q67" s="39"/>
     </row>
@@ -4911,24 +4941,26 @@
       </c>
       <c r="E68" s="34" t="str">
         <f>VLOOKUP(C68,$B$6:$H67,7,FALSE)</f>
-        <v>TBD</v>
+        <v>#1 North Carolina</v>
       </c>
       <c r="F68" s="34" t="str">
         <f>VLOOKUP(D68,$B$6:$H67,7,FALSE)</f>
-        <v>TBD</v>
-      </c>
-      <c r="G68" s="37"/>
+        <v>#2 Villanova</v>
+      </c>
+      <c r="G68" s="37">
+        <v>2</v>
+      </c>
       <c r="H68" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>TBD</v>
-      </c>
-      <c r="J68" s="6" t="str">
+        <v>#2 Villanova</v>
+      </c>
+      <c r="J68" s="6">
         <f>IFERROR(VLOOKUP(E68,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="K68" s="6" t="str">
+        <v>1314</v>
+      </c>
+      <c r="K68" s="6">
         <f>IFERROR(VLOOKUP(F68,teams!$B$2:$C$69,2,FALSE),"")</f>
-        <v/>
+        <v>1437</v>
       </c>
       <c r="M68" s="6" t="str">
         <f t="shared" si="5"/>
@@ -4936,11 +4968,11 @@
       </c>
       <c r="N68" s="6" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>2016_1314_1437</v>
       </c>
       <c r="O68" s="6">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q68" s="39"/>
     </row>
@@ -8040,33 +8072,33 @@
         <f>results!B58</f>
         <v>R3W1</v>
       </c>
-      <c r="B54" s="12" t="str">
+      <c r="B54" s="12">
         <f>IF(results!G54=1,VLOOKUP(results!E54,teams!B$2:C$69,2,FALSE),IF(results!G54=2,VLOOKUP(results!F54,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1242</v>
       </c>
       <c r="C54" s="13" t="str">
         <f>IF(results!G54=1,results!E54,IF(results!G54=2,results!F54,""))</f>
-        <v/>
-      </c>
-      <c r="D54" s="12" t="str">
+        <v>#1 Kansas</v>
+      </c>
+      <c r="D54" s="12">
         <f>IF(results!G54=2,VLOOKUP(results!E54,teams!B$2:C$69,2,FALSE),IF(results!G54=1,VLOOKUP(results!F54,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1268</v>
       </c>
       <c r="E54" s="13" t="str">
         <f>IF(results!G54=2,results!E54,IF(results!G54=1,results!F54,""))</f>
-        <v/>
+        <v>#5 Maryland</v>
       </c>
       <c r="F54" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1242_1268</v>
       </c>
       <c r="G54" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H54" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1242_1268,1</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -8074,33 +8106,33 @@
         <f>results!B59</f>
         <v>R3W2</v>
       </c>
-      <c r="B55" s="12" t="str">
+      <c r="B55" s="12">
         <f>IF(results!G55=1,VLOOKUP(results!E55,teams!B$2:C$69,2,FALSE),IF(results!G55=2,VLOOKUP(results!F55,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1437</v>
       </c>
       <c r="C55" s="13" t="str">
         <f>IF(results!G55=1,results!E55,IF(results!G55=2,results!F55,""))</f>
-        <v/>
-      </c>
-      <c r="D55" s="12" t="str">
+        <v>#2 Villanova</v>
+      </c>
+      <c r="D55" s="12">
         <f>IF(results!G55=2,VLOOKUP(results!E55,teams!B$2:C$69,2,FALSE),IF(results!G55=1,VLOOKUP(results!F55,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1274</v>
       </c>
       <c r="E55" s="13" t="str">
         <f>IF(results!G55=2,results!E55,IF(results!G55=1,results!F55,""))</f>
-        <v/>
+        <v>#3 Miami FL</v>
       </c>
       <c r="F55" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1274_1437</v>
       </c>
       <c r="G55" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H55" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1274_1437,0</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -8108,33 +8140,33 @@
         <f>results!B60</f>
         <v>R3X1</v>
       </c>
-      <c r="B56" s="12" t="str">
+      <c r="B56" s="12">
         <f>IF(results!G56=1,VLOOKUP(results!E56,teams!B$2:C$69,2,FALSE),IF(results!G56=2,VLOOKUP(results!F56,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1332</v>
       </c>
       <c r="C56" s="13" t="str">
         <f>IF(results!G56=1,results!E56,IF(results!G56=2,results!F56,""))</f>
-        <v/>
-      </c>
-      <c r="D56" s="12" t="str">
+        <v>#1 Oregon</v>
+      </c>
+      <c r="D56" s="12">
         <f>IF(results!G56=2,VLOOKUP(results!E56,teams!B$2:C$69,2,FALSE),IF(results!G56=1,VLOOKUP(results!F56,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1181</v>
       </c>
       <c r="E56" s="13" t="str">
         <f>IF(results!G56=2,results!E56,IF(results!G56=1,results!F56,""))</f>
-        <v/>
+        <v>#4 Duke</v>
       </c>
       <c r="F56" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1181_1332</v>
       </c>
       <c r="G56" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H56" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1181_1332,0</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -8142,33 +8174,33 @@
         <f>results!B61</f>
         <v>R3X2</v>
       </c>
-      <c r="B57" s="12" t="str">
+      <c r="B57" s="12">
         <f>IF(results!G57=1,VLOOKUP(results!E57,teams!B$2:C$69,2,FALSE),IF(results!G57=2,VLOOKUP(results!F57,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1328</v>
       </c>
       <c r="C57" s="13" t="str">
         <f>IF(results!G57=1,results!E57,IF(results!G57=2,results!F57,""))</f>
-        <v/>
-      </c>
-      <c r="D57" s="12" t="str">
+        <v>#2 Oklahoma</v>
+      </c>
+      <c r="D57" s="12">
         <f>IF(results!G57=2,VLOOKUP(results!E57,teams!B$2:C$69,2,FALSE),IF(results!G57=1,VLOOKUP(results!F57,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1401</v>
       </c>
       <c r="E57" s="13" t="str">
         <f>IF(results!G57=2,results!E57,IF(results!G57=1,results!F57,""))</f>
-        <v/>
+        <v>#3 Texas A&amp;M</v>
       </c>
       <c r="F57" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1328_1401</v>
       </c>
       <c r="G57" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H57" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1328_1401,1</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -8176,33 +8208,33 @@
         <f>results!B54</f>
         <v>R3Y1</v>
       </c>
-      <c r="B58" s="12" t="str">
+      <c r="B58" s="12">
         <f>IF(results!G58=1,VLOOKUP(results!E58,teams!B$2:C$69,2,FALSE),IF(results!G58=2,VLOOKUP(results!F58,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1314</v>
       </c>
       <c r="C58" s="13" t="str">
         <f>IF(results!G58=1,results!E58,IF(results!G58=2,results!F58,""))</f>
-        <v/>
-      </c>
-      <c r="D58" s="12" t="str">
+        <v>#1 North Carolina</v>
+      </c>
+      <c r="D58" s="12">
         <f>IF(results!G58=2,VLOOKUP(results!E58,teams!B$2:C$69,2,FALSE),IF(results!G58=1,VLOOKUP(results!F58,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1231</v>
       </c>
       <c r="E58" s="13" t="str">
         <f>IF(results!G58=2,results!E58,IF(results!G58=1,results!F58,""))</f>
-        <v/>
+        <v>#5 Indiana</v>
       </c>
       <c r="F58" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1231_1314</v>
       </c>
       <c r="G58" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H58" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1231_1314,0</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -8210,33 +8242,33 @@
         <f>results!B55</f>
         <v>R3Y2</v>
       </c>
-      <c r="B59" s="12" t="str">
+      <c r="B59" s="12">
         <f>IF(results!G59=1,VLOOKUP(results!E59,teams!B$2:C$69,2,FALSE),IF(results!G59=2,VLOOKUP(results!F59,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1323</v>
       </c>
       <c r="C59" s="13" t="str">
         <f>IF(results!G59=1,results!E59,IF(results!G59=2,results!F59,""))</f>
-        <v/>
-      </c>
-      <c r="D59" s="12" t="str">
+        <v>#6 Notre Dame</v>
+      </c>
+      <c r="D59" s="12">
         <f>IF(results!G59=2,VLOOKUP(results!E59,teams!B$2:C$69,2,FALSE),IF(results!G59=1,VLOOKUP(results!F59,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1458</v>
       </c>
       <c r="E59" s="13" t="str">
         <f>IF(results!G59=2,results!E59,IF(results!G59=1,results!F59,""))</f>
-        <v/>
+        <v>#7 Wisconsin</v>
       </c>
       <c r="F59" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1323_1458</v>
       </c>
       <c r="G59" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H59" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1323_1458,1</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -8244,33 +8276,33 @@
         <f>results!B56</f>
         <v>R3Z1</v>
       </c>
-      <c r="B60" s="12" t="str">
+      <c r="B60" s="12">
         <f>IF(results!G60=1,VLOOKUP(results!E60,teams!B$2:C$69,2,FALSE),IF(results!G60=2,VLOOKUP(results!F60,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1438</v>
       </c>
       <c r="C60" s="13" t="str">
         <f>IF(results!G60=1,results!E60,IF(results!G60=2,results!F60,""))</f>
-        <v/>
-      </c>
-      <c r="D60" s="12" t="str">
+        <v>#1 Virginia</v>
+      </c>
+      <c r="D60" s="12">
         <f>IF(results!G60=2,VLOOKUP(results!E60,teams!B$2:C$69,2,FALSE),IF(results!G60=1,VLOOKUP(results!F60,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1235</v>
       </c>
       <c r="E60" s="13" t="str">
         <f>IF(results!G60=2,results!E60,IF(results!G60=1,results!F60,""))</f>
-        <v/>
+        <v>#4 Iowa St</v>
       </c>
       <c r="F60" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1235_1438</v>
       </c>
       <c r="G60" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H60" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1235_1438,0</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -8278,33 +8310,33 @@
         <f>results!B57</f>
         <v>R3Z2</v>
       </c>
-      <c r="B61" s="12" t="str">
+      <c r="B61" s="12">
         <f>IF(results!G61=1,VLOOKUP(results!E61,teams!B$2:C$69,2,FALSE),IF(results!G61=2,VLOOKUP(results!F61,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1393</v>
       </c>
       <c r="C61" s="13" t="str">
         <f>IF(results!G61=1,results!E61,IF(results!G61=2,results!F61,""))</f>
-        <v/>
-      </c>
-      <c r="D61" s="12" t="str">
+        <v>#10 Syracuse</v>
+      </c>
+      <c r="D61" s="12">
         <f>IF(results!G61=2,VLOOKUP(results!E61,teams!B$2:C$69,2,FALSE),IF(results!G61=1,VLOOKUP(results!F61,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1211</v>
       </c>
       <c r="E61" s="13" t="str">
         <f>IF(results!G61=2,results!E61,IF(results!G61=1,results!F61,""))</f>
-        <v/>
+        <v>#11 Gonzaga</v>
       </c>
       <c r="F61" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1211_1393</v>
       </c>
       <c r="G61" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H61" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1211_1393,0</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -8312,33 +8344,33 @@
         <f>results!B64</f>
         <v>R4W1</v>
       </c>
-      <c r="B62" s="12" t="str">
+      <c r="B62" s="12">
         <f>IF(results!G62=1,VLOOKUP(results!E62,teams!B$2:C$69,2,FALSE),IF(results!G62=2,VLOOKUP(results!F62,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1437</v>
       </c>
       <c r="C62" s="13" t="str">
         <f>IF(results!G62=1,results!E62,IF(results!G62=2,results!F62,""))</f>
-        <v/>
-      </c>
-      <c r="D62" s="12" t="str">
+        <v>#2 Villanova</v>
+      </c>
+      <c r="D62" s="12">
         <f>IF(results!G62=2,VLOOKUP(results!E62,teams!B$2:C$69,2,FALSE),IF(results!G62=1,VLOOKUP(results!F62,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1242</v>
       </c>
       <c r="E62" s="13" t="str">
         <f>IF(results!G62=2,results!E62,IF(results!G62=1,results!F62,""))</f>
-        <v/>
+        <v>#1 Kansas</v>
       </c>
       <c r="F62" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1242_1437</v>
       </c>
       <c r="G62" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H62" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1242_1437,0</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -8346,33 +8378,33 @@
         <f>results!B65</f>
         <v>R4X1</v>
       </c>
-      <c r="B63" s="12" t="str">
+      <c r="B63" s="12">
         <f>IF(results!G63=1,VLOOKUP(results!E63,teams!B$2:C$69,2,FALSE),IF(results!G63=2,VLOOKUP(results!F63,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1328</v>
       </c>
       <c r="C63" s="13" t="str">
         <f>IF(results!G63=1,results!E63,IF(results!G63=2,results!F63,""))</f>
-        <v/>
-      </c>
-      <c r="D63" s="12" t="str">
+        <v>#2 Oklahoma</v>
+      </c>
+      <c r="D63" s="12">
         <f>IF(results!G63=2,VLOOKUP(results!E63,teams!B$2:C$69,2,FALSE),IF(results!G63=1,VLOOKUP(results!F63,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1332</v>
       </c>
       <c r="E63" s="13" t="str">
         <f>IF(results!G63=2,results!E63,IF(results!G63=1,results!F63,""))</f>
-        <v/>
+        <v>#1 Oregon</v>
       </c>
       <c r="F63" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1328_1332</v>
       </c>
       <c r="G63" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H63" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1328_1332,1</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -8380,33 +8412,33 @@
         <f>results!B62</f>
         <v>R4Y1</v>
       </c>
-      <c r="B64" s="12" t="str">
+      <c r="B64" s="12">
         <f>IF(results!G64=1,VLOOKUP(results!E64,teams!B$2:C$69,2,FALSE),IF(results!G64=2,VLOOKUP(results!F64,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1314</v>
       </c>
       <c r="C64" s="13" t="str">
         <f>IF(results!G64=1,results!E64,IF(results!G64=2,results!F64,""))</f>
-        <v/>
-      </c>
-      <c r="D64" s="12" t="str">
+        <v>#1 North Carolina</v>
+      </c>
+      <c r="D64" s="12">
         <f>IF(results!G64=2,VLOOKUP(results!E64,teams!B$2:C$69,2,FALSE),IF(results!G64=1,VLOOKUP(results!F64,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1323</v>
       </c>
       <c r="E64" s="13" t="str">
         <f>IF(results!G64=2,results!E64,IF(results!G64=1,results!F64,""))</f>
-        <v/>
+        <v>#6 Notre Dame</v>
       </c>
       <c r="F64" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1314_1323</v>
       </c>
       <c r="G64" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H64" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1314_1323,1</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -8414,33 +8446,33 @@
         <f>results!B63</f>
         <v>R4Z1</v>
       </c>
-      <c r="B65" s="12" t="str">
+      <c r="B65" s="12">
         <f>IF(results!G65=1,VLOOKUP(results!E65,teams!B$2:C$69,2,FALSE),IF(results!G65=2,VLOOKUP(results!F65,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1393</v>
       </c>
       <c r="C65" s="13" t="str">
         <f>IF(results!G65=1,results!E65,IF(results!G65=2,results!F65,""))</f>
-        <v/>
-      </c>
-      <c r="D65" s="12" t="str">
+        <v>#10 Syracuse</v>
+      </c>
+      <c r="D65" s="12">
         <f>IF(results!G65=2,VLOOKUP(results!E65,teams!B$2:C$69,2,FALSE),IF(results!G65=1,VLOOKUP(results!F65,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1438</v>
       </c>
       <c r="E65" s="13" t="str">
         <f>IF(results!G65=2,results!E65,IF(results!G65=1,results!F65,""))</f>
-        <v/>
+        <v>#1 Virginia</v>
       </c>
       <c r="F65" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1393_1438</v>
       </c>
       <c r="G65" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H65" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1393_1438,1</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -8448,33 +8480,33 @@
         <f>results!B66</f>
         <v>R5WX</v>
       </c>
-      <c r="B66" s="12" t="str">
+      <c r="B66" s="12">
         <f>IF(results!G66=1,VLOOKUP(results!E66,teams!B$2:C$69,2,FALSE),IF(results!G66=2,VLOOKUP(results!F66,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1314</v>
       </c>
       <c r="C66" s="13" t="str">
         <f>IF(results!G66=1,results!E66,IF(results!G66=2,results!F66,""))</f>
-        <v/>
-      </c>
-      <c r="D66" s="12" t="str">
+        <v>#1 North Carolina</v>
+      </c>
+      <c r="D66" s="12">
         <f>IF(results!G66=2,VLOOKUP(results!E66,teams!B$2:C$69,2,FALSE),IF(results!G66=1,VLOOKUP(results!F66,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1393</v>
       </c>
       <c r="E66" s="13" t="str">
         <f>IF(results!G66=2,results!E66,IF(results!G66=1,results!F66,""))</f>
-        <v/>
+        <v>#10 Syracuse</v>
       </c>
       <c r="F66" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2015_1314_1393</v>
       </c>
       <c r="G66" s="13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H66" s="13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2015_1314_1393,1</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -8482,33 +8514,33 @@
         <f>results!B67</f>
         <v>R5YZ</v>
       </c>
-      <c r="B67" s="12" t="str">
+      <c r="B67" s="12">
         <f>IF(results!G67=1,VLOOKUP(results!E67,teams!B$2:C$69,2,FALSE),IF(results!G67=2,VLOOKUP(results!F67,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1437</v>
       </c>
       <c r="C67" s="13" t="str">
         <f>IF(results!G67=1,results!E67,IF(results!G67=2,results!F67,""))</f>
-        <v/>
-      </c>
-      <c r="D67" s="12" t="str">
+        <v>#2 Villanova</v>
+      </c>
+      <c r="D67" s="12">
         <f>IF(results!G67=2,VLOOKUP(results!E67,teams!B$2:C$69,2,FALSE),IF(results!G67=1,VLOOKUP(results!F67,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1328</v>
       </c>
       <c r="E67" s="13" t="str">
         <f>IF(results!G67=2,results!E67,IF(results!G67=1,results!F67,""))</f>
-        <v/>
+        <v>#2 Oklahoma</v>
       </c>
       <c r="F67" s="13" t="str">
         <f t="shared" ref="F67:F68" si="6">IF(B67=D67,"",IF(B67&lt;D67,"2015_"&amp;B67&amp;"_"&amp;D67,"2015_"&amp;D67&amp;"_"&amp;B67))</f>
-        <v/>
+        <v>2015_1328_1437</v>
       </c>
       <c r="G67" s="13" t="str">
         <f t="shared" ref="G67:G68" si="7">IF(B67=D67,"",IF(B67&lt;D67,"1","0"))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H67" s="13" t="str">
         <f t="shared" ref="H67:H68" si="8">IF(B67=D67,"",IF(B67&lt;D67,"2015_"&amp;B67&amp;"_"&amp;D67&amp;",1","2015_"&amp;D67&amp;"_"&amp;B67&amp;",0"))</f>
-        <v/>
+        <v>2015_1328_1437,0</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -8516,33 +8548,33 @@
         <f>results!B68</f>
         <v>R6CH</v>
       </c>
-      <c r="B68" s="12" t="str">
+      <c r="B68" s="12">
         <f>IF(results!G68=1,VLOOKUP(results!E68,teams!B$2:C$69,2,FALSE),IF(results!G68=2,VLOOKUP(results!F68,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1437</v>
       </c>
       <c r="C68" s="13" t="str">
         <f>IF(results!G68=1,results!E68,IF(results!G68=2,results!F68,""))</f>
-        <v/>
-      </c>
-      <c r="D68" s="12" t="str">
+        <v>#2 Villanova</v>
+      </c>
+      <c r="D68" s="12">
         <f>IF(results!G68=2,VLOOKUP(results!E68,teams!B$2:C$69,2,FALSE),IF(results!G68=1,VLOOKUP(results!F68,teams!B$2:C$69,2,FALSE),""))</f>
-        <v/>
+        <v>1314</v>
       </c>
       <c r="E68" s="13" t="str">
         <f>IF(results!G68=2,results!E68,IF(results!G68=1,results!F68,""))</f>
-        <v/>
+        <v>#1 North Carolina</v>
       </c>
       <c r="F68" s="13" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>2015_1314_1437</v>
       </c>
       <c r="G68" s="13" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H68" s="13" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>2015_1314_1437,0</v>
       </c>
     </row>
   </sheetData>
@@ -9318,7 +9350,7 @@
       </c>
       <c r="C54">
         <f>results!O54</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -9332,7 +9364,7 @@
       </c>
       <c r="C55">
         <f>results!O55</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -9346,7 +9378,7 @@
       </c>
       <c r="C56">
         <f>results!O56</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -9360,7 +9392,7 @@
       </c>
       <c r="C57">
         <f>results!O57</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -9374,7 +9406,7 @@
       </c>
       <c r="C58">
         <f>results!O58</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -9388,7 +9420,7 @@
       </c>
       <c r="C59">
         <f>results!O59</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -9402,7 +9434,7 @@
       </c>
       <c r="C60">
         <f>results!O60</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -9416,7 +9448,7 @@
       </c>
       <c r="C61">
         <f>results!O61</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -9426,11 +9458,11 @@
       </c>
       <c r="B62" t="str">
         <f>results!N62</f>
-        <v/>
+        <v>2016_1242_1437</v>
       </c>
       <c r="C62">
         <f>results!O62</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -9440,11 +9472,11 @@
       </c>
       <c r="B63" t="str">
         <f>results!N63</f>
-        <v/>
+        <v>2016_1328_1332</v>
       </c>
       <c r="C63">
         <f>results!O63</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -9454,11 +9486,11 @@
       </c>
       <c r="B64" t="str">
         <f>results!N64</f>
-        <v/>
+        <v>2016_1314_1323</v>
       </c>
       <c r="C64">
         <f>results!O64</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -9468,11 +9500,11 @@
       </c>
       <c r="B65" t="str">
         <f>results!N65</f>
-        <v/>
+        <v>2016_1393_1438</v>
       </c>
       <c r="C65">
         <f>results!O65</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -9482,11 +9514,11 @@
       </c>
       <c r="B66" t="str">
         <f>results!N66</f>
-        <v/>
+        <v>2016_1314_1393</v>
       </c>
       <c r="C66">
         <f>results!O66</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -9496,11 +9528,11 @@
       </c>
       <c r="B67" t="str">
         <f>results!N67</f>
-        <v/>
+        <v>2016_1328_1437</v>
       </c>
       <c r="C67">
         <f>results!O67</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -9510,11 +9542,11 @@
       </c>
       <c r="B68" t="str">
         <f>results!N68</f>
-        <v/>
+        <v>2016_1314_1437</v>
       </c>
       <c r="C68">
         <f>results!O68</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>